<commit_message>
Committing newly added features and corresponding steps on Class module
</commit_message>
<xml_diff>
--- a/Playwright_Group5_LMS_BDD_Project/tests/TestData/PlayWright_Group5_Data.xlsx
+++ b/Playwright_Group5_LMS_BDD_Project/tests/TestData/PlayWright_Group5_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amreennaziasyed/Playwright_Group2_LMS_BDD_Project/tests/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VijayaBharati_Playwright\Group5_Playwrighters\Playwrighters_LMS_project\Playwright_Group5_LMS_BDD_Project\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EDE296-3FF4-AC4B-85C7-E7359EB654A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA75E1D-FBC7-42C4-B66D-86AD76641F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -162,15 +162,9 @@
     <t>staffName</t>
   </si>
   <si>
-    <t>SMPO-0001</t>
-  </si>
-  <si>
     <t>arunasel S</t>
   </si>
   <si>
-    <t>Scrum master</t>
-  </si>
-  <si>
     <t>editprogram</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>Saranya M</t>
   </si>
   <si>
-    <t>ClassDesc</t>
-  </si>
-  <si>
     <t>OptionalValid</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>c:/Recordings</t>
   </si>
   <si>
-    <t>Recording</t>
-  </si>
-  <si>
     <t>NumericOrAlphaData</t>
   </si>
   <si>
@@ -232,6 +220,30 @@
   </si>
   <si>
     <t>marketing</t>
+  </si>
+  <si>
+    <t>Class Description</t>
+  </si>
+  <si>
+    <t>Class recordings</t>
+  </si>
+  <si>
+    <t>Important notes</t>
+  </si>
+  <si>
+    <t>Test comments</t>
+  </si>
+  <si>
+    <t>classDesc</t>
+  </si>
+  <si>
+    <t>Recordings</t>
+  </si>
+  <si>
+    <t>Java Batch 01</t>
+  </si>
+  <si>
+    <t>Playwrighters three</t>
   </si>
 </sst>
 </file>
@@ -316,9 +328,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -356,7 +368,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -462,7 +474,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -604,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -618,15 +630,15 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -640,7 +652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -651,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -665,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -679,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -690,7 +702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -704,7 +716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -731,15 +743,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -756,7 +768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -770,7 +782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -784,7 +796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -801,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -818,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -835,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -861,20 +873,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE17ACF-C6C7-40F7-BE92-0D5B7CEEB2BA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
     <col min="3" max="4" width="42" style="3" customWidth="1"/>
     <col min="5" max="5" width="28" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="3"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -885,13 +897,13 @@
         <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -902,40 +914,40 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -948,19 +960,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9E0E79-7EE5-814B-B938-A957080C7691}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -974,60 +990,72 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>51</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>23423</v>

</xml_diff>

<commit_message>
Adding few changes made in Class Steps and test data
</commit_message>
<xml_diff>
--- a/Playwright_Group5_LMS_BDD_Project/tests/TestData/PlayWright_Group5_Data.xlsx
+++ b/Playwright_Group5_LMS_BDD_Project/tests/TestData/PlayWright_Group5_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VijayaBharati_Playwright\Group5_Playwrighters\Playwrighters_LMS_project\Playwright_Group5_LMS_BDD_Project\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA75E1D-FBC7-42C4-B66D-86AD76641F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6DDA54-7E5E-4836-B471-75BFB30ACE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -180,9 +180,6 @@
     <t>ValidEditData</t>
   </si>
   <si>
-    <t>Saranya M</t>
-  </si>
-  <si>
     <t>OptionalValid</t>
   </si>
   <si>
@@ -243,7 +240,13 @@
     <t>Java Batch 01</t>
   </si>
   <si>
-    <t>Playwrighters three</t>
+    <t>Kevin Thomas</t>
+  </si>
+  <si>
+    <t>Playwrighters team four</t>
+  </si>
+  <si>
+    <t>updated Playwrighters</t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
         <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -930,16 +933,16 @@
         <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -947,7 +950,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -961,14 +964,14 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
@@ -990,16 +993,16 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
         <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1007,7 +1010,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -1016,46 +1019,49 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
         <v>52</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5">
         <v>23423</v>

</xml_diff>